<commit_message>
app and device manager
</commit_message>
<xml_diff>
--- a/Skins/details.xlsx
+++ b/Skins/details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>label</t>
   </si>
@@ -178,6 +178,22 @@
   </si>
   <si>
     <t>C:\Program Files\Adobe\Adobe Photoshop CS6 (64 Bit)\Photoshop.exe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shell:::{74246bfc-4c96-11d0-abef-0020af6b0b7a}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell:::{7b81be6a-ce2b-4676-a29e-eb907a5126c5}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -505,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +798,34 @@
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>